<commit_message>
starting devt for list conversions. added 2 files, and fixed alignments in header
</commit_message>
<xml_diff>
--- a/pdfs/ASM Corewar - v.1.1.xlsx
+++ b/pdfs/ASM Corewar - v.1.1.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="51200" yWindow="4800" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Core War" sheetId="1" r:id="rId1"/>
+    <sheet name="Commands Table" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -865,19 +865,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -895,25 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1199,7 +1199,7 @@
   <dimension ref="A1:M1054"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1219,35 +1219,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="71"/>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="2" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
       <c r="M2" s="60"/>
     </row>
     <row r="3" spans="1:13" ht="26" x14ac:dyDescent="0.15">
@@ -1396,7 +1396,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="104" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="78" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>4</v>
       </c>
@@ -1928,16 +1928,16 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
       <c r="K24" s="33" t="s">
@@ -1963,7 +1963,7 @@
       <c r="F25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G25" s="73" t="s">
+      <c r="G25" s="66" t="s">
         <v>6</v>
       </c>
       <c r="H25" s="60"/>
@@ -1992,7 +1992,7 @@
       <c r="F26" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G26" s="57" t="s">
+      <c r="G26" s="59" t="s">
         <v>99</v>
       </c>
       <c r="H26" s="60"/>
@@ -2015,7 +2015,7 @@
       <c r="F27" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="68" t="s">
+      <c r="G27" s="65" t="s">
         <v>102</v>
       </c>
       <c r="H27" s="60"/>
@@ -2040,7 +2040,7 @@
       <c r="F28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="57" t="s">
+      <c r="G28" s="59" t="s">
         <v>105</v>
       </c>
       <c r="H28" s="60"/>
@@ -2059,10 +2059,10 @@
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
-      <c r="G29" s="70" t="s">
+      <c r="G29" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="H29" s="67"/>
+      <c r="H29" s="58"/>
       <c r="I29" s="34"/>
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
@@ -2099,15 +2099,15 @@
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" ht="34" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="61" t="s">
+      <c r="A32" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="1"/>
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
@@ -2123,11 +2123,11 @@
         <v>109</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="62" t="s">
+      <c r="D33" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="59"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="64"/>
       <c r="G33" s="60"/>
       <c r="H33" s="45"/>
       <c r="I33" s="34"/>
@@ -2144,11 +2144,11 @@
         <v>50</v>
       </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="57" t="s">
+      <c r="D34" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="59"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="64"/>
       <c r="G34" s="60"/>
       <c r="H34" s="45"/>
       <c r="I34" s="34"/>
@@ -2165,11 +2165,11 @@
         <v>50</v>
       </c>
       <c r="C35" s="14"/>
-      <c r="D35" s="68" t="s">
+      <c r="D35" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="E35" s="69"/>
-      <c r="F35" s="59"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="64"/>
       <c r="G35" s="60"/>
       <c r="H35" s="45"/>
       <c r="I35" s="34"/>
@@ -2186,12 +2186,12 @@
         <v>115</v>
       </c>
       <c r="C36" s="50"/>
-      <c r="D36" s="64" t="s">
+      <c r="D36" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="65"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="67"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="45"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
@@ -17438,6 +17438,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D35:G35"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="A1:M1"/>
@@ -17446,11 +17451,6 @@
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>